<commit_message>
files for class on 9/6/2017
</commit_message>
<xml_diff>
--- a/moredata.xlsx
+++ b/moredata.xlsx
@@ -375,12 +375,12 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="11.53125" customWidth="1"/>
+    <col min="4" max="4" width="12.9296875" customWidth="1"/>
     <col min="5" max="5" width="11.1328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -486,7 +486,7 @@
       <c r="C5">
         <v>200</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="1">

</xml_diff>